<commit_message>
Updated master references for IG 1.0.3
</commit_message>
<xml_diff>
--- a/doc/message/common/OIOXML FHIR references.xlsx
+++ b/doc/message/common/OIOXML FHIR references.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10314"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/MedCom/drafts/Standarder/HL7/FHIR/HospitalNotification/Baggrundsmateriale/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC874FE-1523-B54A-BF30-A7FEA7AE4C92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316499EF-35AF-F14A-AE59-171250A7952A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="1220" windowWidth="34520" windowHeight="24880" tabRatio="272" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10160" yWindow="3920" windowWidth="34820" windowHeight="26720" tabRatio="272" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HospitalNotification" sheetId="1" r:id="rId1"/>
-    <sheet name="ClinicalEmail" sheetId="6" r:id="rId2"/>
+    <sheet name="CareCommunication" sheetId="6" r:id="rId2"/>
     <sheet name="temp" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ClinicalEmail!$A$1:$F$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">CareCommunication!$A$1:$F$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">HospitalNotification!$A$1:$F$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">temp!$A$1:$F$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">ClinicalEmail!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">CareCommunication!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">HospitalNotification!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">temp!$3:$3</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="162">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -112,9 +112,6 @@
     <t>Sender/receiver id</t>
   </si>
   <si>
-    <t>In FHIR always SOR</t>
-  </si>
-  <si>
     <t>Sender/receiver type</t>
   </si>
   <si>
@@ -175,27 +172,12 @@
     <t>Bundle.entry.MedComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.MedComMessagingOrganization.identifier.EANIdentifier</t>
   </si>
   <si>
-    <t>Bundle.entry.MedComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.MedComMessagingOrganization.identifier.sorIdentifier</t>
-  </si>
-  <si>
-    <t>Bundle.entry.MedComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.MedComMessagingOrganization.address.text</t>
-  </si>
-  <si>
-    <t>Bundle.entry.MedComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.MedComMessagingOrganization.telecom</t>
-  </si>
-  <si>
     <t>Notification start date</t>
   </si>
   <si>
     <t>Notification  start time</t>
   </si>
   <si>
-    <t>The department is identified by SOR id</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Emesssage.ClinicalEmail.Letter.StatisticalCode</t>
   </si>
   <si>
@@ -244,18 +226,12 @@
     <t>Emesssage.ClinicalEmail.&lt;sender/receiver&gt;.StreetName</t>
   </si>
   <si>
-    <t>Bundle.entry.MedComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.MedComMessagingOrganization.address.line</t>
-  </si>
-  <si>
     <t>Medical speciality code</t>
   </si>
   <si>
     <t>Emesssage.ClinicalEmail.sender.MedicalSpecialityCode</t>
   </si>
   <si>
-    <t>Department is identified by SOR and this information is expected to be expressed in SOR</t>
-  </si>
-  <si>
     <t>Patient alternative id</t>
   </si>
   <si>
@@ -328,9 +304,6 @@
     <t>Emessage.ClinicalEmail.Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Bundle.entry.MedComMessagingMessageHeader.MedComClinicalCommunication.sender.sorid </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bundle.entry.MedComMessagingMessageHeader.MedComClinicalCommunication.payload.Attachment </t>
   </si>
   <si>
@@ -382,24 +355,9 @@
     <t>Bundle.medComMessagingMessageHeader.medComHospitalNotificationEncounter.episodeOfCare.identifier.value</t>
   </si>
   <si>
-    <t>Bundle.medComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.medComMessagingOrganization.identifier.sorIdentifier</t>
-  </si>
-  <si>
     <t>Bundle.medComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.medComMessagingOrganization.identifier.EANIdentifier</t>
   </si>
   <si>
-    <t>Bundle.medComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.medComMessagingOrganization.address.text</t>
-  </si>
-  <si>
-    <t>The unit  is identified by SOR id</t>
-  </si>
-  <si>
-    <t>Bundle.medComMessagingMessageHeader.medCom.hospitalNotificationEncounter.serviceProvider.reference</t>
-  </si>
-  <si>
-    <t>Bundle.medComMessagingMessageHeader.&lt;destination.primary.receiver/sender&gt;.medComMessagingOrganization.telecom</t>
-  </si>
-  <si>
     <t>Bundle.medComMessagingMessageHeader.medComHospitalNotificationEncounter.medComCorePatient.identifier.cpr</t>
   </si>
   <si>
@@ -448,9 +406,6 @@
     <t>Bundle.medcomMessagingMessage.event.eventcoding</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bundle.medcomMessagingMessage.event.eventcoding</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Bundle.medComMessagingMessageHeader.medComHospitalNotificationEncounter.class and Bundle.medComMessagingMessageHeader.medComHospitalNotificationEncounter.status</t>
   </si>
   <si>
@@ -523,14 +478,65 @@
     <t>Bundle.entry.MedComMessagingMessageHeader.MedComClinicalCommunication.MedComCoreEncounter.EpisodeOfCare.identifier</t>
   </si>
   <si>
-    <t>Only VANSEnvelope contains stastical code.</t>
+    <t>MedComMessagingOrganization</t>
+  </si>
+  <si>
+    <t>Bundle.medComMessagingMessageHeader..extension:reportOfAdmissionFlag</t>
+  </si>
+  <si>
+    <t>Department is either  referenced via SOR of EAN by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t>Unitname is either  referenced via SOR of EAN by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t>Telephonenumber is either  referenced via SOR of EAN by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t>OrganizationName is either  referenced via SOR of EAN by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t>Identifier is either a SOR or EAN identifier referenced by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t>The version of the FHIR profiles is part of all  the Profile url, and is presenty 1.0, eg. http://medcomfhir.dk/fhir/core/1.0/StructureDefinition/medcom-hospitalNotification-message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only VANSEnvelope contains stastical code. For HosptalNotification the Statistical Code is FDIS20 </t>
+  </si>
+  <si>
+    <t>For HosptialNotification the code is "hospital-notification-message"</t>
+  </si>
+  <si>
+    <t>The Identifier that corresponds to the NotificationIdentifier.</t>
+  </si>
+  <si>
+    <t>The version of the FHIR profiles is part of all  the Profile url, and is presenty 1.0, eg. http://medcomfhir.dk/fhir/core/1.0/StructureDefinition/medcom-carecommunication-message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only VANSEnvelope contains stastical code. For HosptalNotification the Statistical Code is FDIS91 </t>
+  </si>
+  <si>
+    <t>For CareCommunication it is care-communication-message</t>
+  </si>
+  <si>
+    <t>Steetname is either  referenced via SOR of EAN by  Bundle.medComMessagingMessageHeader.Encounter.serviceProvider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In FHIR the encounter references a SOR or EAN organization. The type  of organization is defined by the code system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Identifier for alternative person identification will have a code system that reflects this  </t>
+  </si>
+  <si>
+    <t>Bundle.medComMessagingMessageHeader.MedComHospitalNotificationReportOfAdmissionRecipientExtension</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -616,11 +622,6 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial (Body)"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial (Body)"/>
     </font>
     <font>
@@ -730,9 +731,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -742,13 +740,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1333,8 +1334,8 @@
   </sheetPr>
   <dimension ref="B1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="123" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="123" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1383,10 +1384,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="26" x14ac:dyDescent="0.15">
@@ -1397,7 +1398,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1409,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1432,88 +1433,88 @@
         <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:6" ht="52" x14ac:dyDescent="0.15">
       <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>49</v>
+        <v>139</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>159</v>
+      <c r="E10" s="14" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B13" s="8" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>0</v>
@@ -1521,165 +1522,173 @@
     </row>
     <row r="15" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="6"/>
+      <c r="C16" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="17" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>146</v>
+      <c r="C17" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5" ht="14" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="39" x14ac:dyDescent="0.15">
       <c r="B18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>145</v>
+        <v>22</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>130</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:5" ht="26" x14ac:dyDescent="0.15">
+      <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="26" x14ac:dyDescent="0.15">
+      <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>142</v>
+      <c r="C21" s="17" t="s">
+        <v>127</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>141</v>
+        <v>26</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>140</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>161</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B24" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5" ht="52" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:5" ht="26" x14ac:dyDescent="0.15">
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -1687,13 +1696,13 @@
     </row>
     <row r="28" spans="2:5" ht="28" x14ac:dyDescent="0.15">
       <c r="B28" s="8" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="E28" s="7"/>
     </row>
@@ -1721,8 +1730,8 @@
   </sheetPr>
   <dimension ref="B1:F42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1745,7 +1754,7 @@
     </row>
     <row r="2" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1763,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="26" x14ac:dyDescent="0.15">
@@ -1774,14 +1783,14 @@
         <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1789,7 +1798,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="9"/>
@@ -1802,7 +1811,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="9"/>
@@ -1827,351 +1836,357 @@
         <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:6" ht="78" x14ac:dyDescent="0.15">
       <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:6" ht="52" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>159</v>
+      <c r="E10" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="2:6" ht="28" x14ac:dyDescent="0.15">
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>132</v>
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="2:6" ht="28" x14ac:dyDescent="0.15">
       <c r="B12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B13" s="8" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="B15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="2:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="B15" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="2:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="2:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="7"/>
+        <v>150</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>0</v>
+      </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="2:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:6" ht="52" x14ac:dyDescent="0.15">
       <c r="B18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:6" ht="28" x14ac:dyDescent="0.15">
       <c r="B19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>44</v>
+        <v>53</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>146</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B21" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>48</v>
+        <v>147</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B22" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="2:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B24" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B25" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:6" ht="39" x14ac:dyDescent="0.15">
       <c r="B26" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B27" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B28" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B30" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B31" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B32" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B33" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2180,69 +2195,69 @@
     </row>
     <row r="34" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>123</v>
+        <v>29</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>136</v>
+        <v>120</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B36" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>97</v>
-      </c>
       <c r="E36" s="9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B37" s="8" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B38" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>0</v>
@@ -2251,39 +2266,39 @@
     </row>
     <row r="39" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B39" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="2:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B40" s="8" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>124</v>
+      <c r="D40" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="2:6" ht="26" x14ac:dyDescent="0.15">
       <c r="B41" s="8" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>125</v>
+      <c r="D41" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="9"/>
@@ -2382,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>

</xml_diff>